<commit_message>
Updated the User list and listserv
</commit_message>
<xml_diff>
--- a/Janelia Workstation User List.xlsx
+++ b/Janelia Workstation User List.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13420" windowHeight="20240" tabRatio="500"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="242">
   <si>
     <t>bukowinskip</t>
   </si>
@@ -731,6 +731,21 @@
   </si>
   <si>
     <t xml:space="preserve">Visiting Scientist </t>
+  </si>
+  <si>
+    <t>sitaramand</t>
+  </si>
+  <si>
+    <t>ihrkeg</t>
+  </si>
+  <si>
+    <t>Gudrun Ihrke</t>
+  </si>
+  <si>
+    <t>Divya Sitaraman</t>
+  </si>
+  <si>
+    <t>Enter full info in Subject table</t>
   </si>
 </sst>
 </file>
@@ -846,12 +861,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="110">
+  <cellStyleXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -979,7 +1010,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="110">
+  <cellStyles count="126">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -1037,6 +1068,14 @@
     <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
@@ -1089,6 +1128,14 @@
     <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1418,10 +1465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I114"/>
+  <dimension ref="A1:I116"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D114" sqref="D114"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1440,17 +1487,19 @@
         <v>156</v>
       </c>
       <c r="B1" s="4">
-        <v>40253</v>
+        <v>40267</v>
       </c>
       <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="E1" s="5" t="s">
+        <v>180</v>
+      </c>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:9">
       <c r="D2" s="6"/>
-      <c r="E2" s="5" t="s">
-        <v>180</v>
+      <c r="E2" t="s">
+        <v>168</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -1461,7 +1510,7 @@
       </c>
       <c r="D3" s="6"/>
       <c r="E3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
@@ -1472,7 +1521,7 @@
       </c>
       <c r="D4" s="6"/>
       <c r="E4" t="s">
-        <v>167</v>
+        <v>241</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -2137,10 +2186,10 @@
         <v>210</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>47</v>
+        <v>238</v>
       </c>
       <c r="H35" t="s">
-        <v>96</v>
+        <v>239</v>
       </c>
       <c r="I35" t="s">
         <v>142</v>
@@ -2160,13 +2209,13 @@
         <v>139</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="H36" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I36" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -2183,13 +2232,13 @@
         <v>140</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="H37" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I37" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -2206,13 +2255,13 @@
         <v>141</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>62</v>
+        <v>5</v>
       </c>
       <c r="H38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I38" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -2220,19 +2269,19 @@
         <v>45</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>47</v>
+        <v>238</v>
       </c>
       <c r="D39" t="s">
-        <v>96</v>
+        <v>239</v>
       </c>
       <c r="E39" t="s">
         <v>142</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="H39" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I39" t="s">
         <v>142</v>
@@ -2243,19 +2292,19 @@
         <v>57</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="D40" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E40" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="H40" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I40" t="s">
         <v>142</v>
@@ -2263,134 +2312,134 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="1" t="s">
-        <v>47</v>
+        <v>238</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="D41" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E41" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>191</v>
+        <v>71</v>
       </c>
       <c r="H41" t="s">
-        <v>217</v>
+        <v>101</v>
       </c>
       <c r="I41" t="s">
-        <v>211</v>
+        <v>142</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="1" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>62</v>
+        <v>5</v>
       </c>
       <c r="D42" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E42" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>40</v>
+        <v>191</v>
       </c>
       <c r="H42" t="s">
-        <v>102</v>
+        <v>217</v>
       </c>
       <c r="I42" t="s">
-        <v>136</v>
+        <v>211</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="1" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="D43" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E43" t="s">
         <v>142</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>157</v>
+        <v>40</v>
       </c>
       <c r="H43" t="s">
-        <v>162</v>
+        <v>102</v>
       </c>
       <c r="I43" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="1" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="D44" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E44" t="s">
         <v>142</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>30</v>
+        <v>157</v>
       </c>
       <c r="H44" t="s">
-        <v>103</v>
+        <v>162</v>
       </c>
       <c r="I44" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="1" t="s">
-        <v>62</v>
+        <v>5</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>191</v>
+        <v>71</v>
       </c>
       <c r="D45" t="s">
-        <v>217</v>
+        <v>101</v>
       </c>
       <c r="E45" t="s">
-        <v>211</v>
+        <v>142</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H45" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I45" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>40</v>
+        <v>191</v>
       </c>
       <c r="D46" t="s">
-        <v>102</v>
+        <v>217</v>
       </c>
       <c r="E46" t="s">
-        <v>136</v>
+        <v>211</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="H46" t="s">
         <v>104</v>
@@ -2401,22 +2450,22 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="1" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>157</v>
+        <v>40</v>
       </c>
       <c r="D47" t="s">
-        <v>162</v>
+        <v>102</v>
       </c>
       <c r="E47" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="H47" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I47" t="s">
         <v>141</v>
@@ -2424,56 +2473,56 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="1" t="s">
-        <v>191</v>
+        <v>71</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>30</v>
+        <v>157</v>
       </c>
       <c r="D48" t="s">
-        <v>103</v>
+        <v>162</v>
       </c>
       <c r="E48" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>204</v>
+        <v>53</v>
       </c>
       <c r="H48" t="s">
-        <v>232</v>
+        <v>105</v>
       </c>
       <c r="I48" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="1" t="s">
-        <v>15</v>
+        <v>191</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D49" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E49" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>186</v>
+        <v>204</v>
       </c>
       <c r="H49" t="s">
-        <v>213</v>
+        <v>232</v>
       </c>
       <c r="I49" t="s">
-        <v>209</v>
+        <v>142</v>
       </c>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="1" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="D50" t="s">
         <v>104</v>
@@ -2482,33 +2531,33 @@
         <v>141</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>59</v>
+        <v>186</v>
       </c>
       <c r="H50" t="s">
-        <v>106</v>
+        <v>213</v>
       </c>
       <c r="I50" t="s">
-        <v>141</v>
+        <v>209</v>
       </c>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="1" t="s">
-        <v>157</v>
+        <v>40</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="D51" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E51" t="s">
         <v>141</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="H51" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I51" t="s">
         <v>141</v>
@@ -2516,22 +2565,22 @@
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="1" t="s">
-        <v>30</v>
+        <v>157</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>204</v>
+        <v>53</v>
       </c>
       <c r="D52" t="s">
-        <v>232</v>
+        <v>105</v>
       </c>
       <c r="E52" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="H52" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I52" t="s">
         <v>141</v>
@@ -2539,114 +2588,114 @@
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="1" t="s">
-        <v>158</v>
+        <v>30</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>186</v>
+        <v>204</v>
       </c>
       <c r="D53" t="s">
-        <v>213</v>
+        <v>232</v>
       </c>
       <c r="E53" t="s">
-        <v>209</v>
+        <v>142</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>206</v>
+        <v>60</v>
       </c>
       <c r="H53" t="s">
-        <v>234</v>
+        <v>108</v>
       </c>
       <c r="I53" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" s="1" t="s">
-        <v>34</v>
+        <v>158</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>59</v>
+        <v>186</v>
       </c>
       <c r="D54" t="s">
-        <v>106</v>
+        <v>213</v>
       </c>
       <c r="E54" t="s">
-        <v>141</v>
+        <v>209</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>46</v>
+        <v>206</v>
       </c>
       <c r="H54" t="s">
-        <v>109</v>
+        <v>234</v>
       </c>
       <c r="I54" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="1" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="D55" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E55" t="s">
         <v>141</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>201</v>
+        <v>46</v>
       </c>
       <c r="H55" t="s">
-        <v>228</v>
+        <v>109</v>
       </c>
       <c r="I55" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="1" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="D56" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E56" t="s">
         <v>141</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="H56" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="I56" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="1" t="s">
-        <v>204</v>
+        <v>53</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>206</v>
+        <v>60</v>
       </c>
       <c r="D57" t="s">
-        <v>234</v>
+        <v>108</v>
       </c>
       <c r="E57" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>2</v>
+        <v>205</v>
       </c>
       <c r="H57" t="s">
-        <v>110</v>
+        <v>233</v>
       </c>
       <c r="I57" t="s">
         <v>142</v>
@@ -2654,68 +2703,68 @@
     </row>
     <row r="58" spans="1:9">
       <c r="A58" s="1" t="s">
-        <v>186</v>
+        <v>204</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>46</v>
+        <v>206</v>
       </c>
       <c r="D58" t="s">
-        <v>109</v>
+        <v>234</v>
       </c>
       <c r="E58" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>69</v>
+        <v>2</v>
       </c>
       <c r="H58" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I58" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" s="1" t="s">
-        <v>56</v>
+        <v>186</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>201</v>
+        <v>46</v>
       </c>
       <c r="D59" t="s">
-        <v>228</v>
+        <v>109</v>
       </c>
       <c r="E59" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>4</v>
+        <v>69</v>
       </c>
       <c r="H59" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I59" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" s="1" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D60" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="E60" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>77</v>
+        <v>4</v>
       </c>
       <c r="H60" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I60" t="s">
         <v>129</v>
@@ -2723,272 +2772,272 @@
     </row>
     <row r="61" spans="1:9">
       <c r="A61" s="1" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>2</v>
+        <v>205</v>
       </c>
       <c r="D61" t="s">
-        <v>110</v>
+        <v>233</v>
       </c>
       <c r="E61" t="s">
         <v>142</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>173</v>
+        <v>77</v>
       </c>
       <c r="H61" t="s">
-        <v>174</v>
+        <v>113</v>
       </c>
       <c r="I61" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" s="1" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>69</v>
+        <v>2</v>
       </c>
       <c r="D62" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E62" t="s">
+        <v>142</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="H62" t="s">
+        <v>174</v>
+      </c>
+      <c r="I62" t="s">
         <v>131</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H62" t="s">
-        <v>114</v>
-      </c>
-      <c r="I62" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="63" spans="1:9">
       <c r="A63" s="1" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>4</v>
+        <v>69</v>
       </c>
       <c r="D63" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E63" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="H63" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I63" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" s="1" t="s">
-        <v>206</v>
+        <v>60</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>77</v>
+        <v>4</v>
       </c>
       <c r="D64" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E64" t="s">
         <v>129</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="H64" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I64" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
     <row r="65" spans="1:9">
       <c r="A65" s="1" t="s">
-        <v>46</v>
+        <v>206</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>173</v>
+        <v>77</v>
       </c>
       <c r="D65" t="s">
-        <v>174</v>
+        <v>113</v>
       </c>
       <c r="E65" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="H65" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I65" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
     </row>
     <row r="66" spans="1:9">
       <c r="A66" s="1" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>18</v>
+        <v>173</v>
       </c>
       <c r="D66" t="s">
-        <v>114</v>
+        <v>174</v>
       </c>
       <c r="E66" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>192</v>
+        <v>17</v>
       </c>
       <c r="H66" t="s">
-        <v>218</v>
+        <v>117</v>
       </c>
       <c r="I66" t="s">
-        <v>211</v>
+        <v>129</v>
       </c>
     </row>
     <row r="67" spans="1:9">
       <c r="A67" s="1" t="s">
-        <v>201</v>
+        <v>23</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="D67" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E67" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>26</v>
+        <v>192</v>
       </c>
       <c r="H67" t="s">
-        <v>118</v>
+        <v>218</v>
       </c>
       <c r="I67" t="s">
-        <v>141</v>
+        <v>211</v>
       </c>
     </row>
     <row r="68" spans="1:9">
       <c r="A68" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="D68" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E68" t="s">
+        <v>145</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H68" t="s">
+        <v>118</v>
+      </c>
+      <c r="I68" t="s">
         <v>141</v>
-      </c>
-      <c r="G68" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H68" t="s">
-        <v>119</v>
-      </c>
-      <c r="I68" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="69" spans="1:9">
       <c r="A69" s="1" t="s">
-        <v>14</v>
+        <v>205</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="D69" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E69" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>187</v>
+        <v>43</v>
       </c>
       <c r="H69" t="s">
-        <v>214</v>
+        <v>119</v>
       </c>
       <c r="I69" t="s">
-        <v>209</v>
+        <v>136</v>
       </c>
     </row>
     <row r="70" spans="1:9">
       <c r="A70" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>192</v>
+        <v>17</v>
       </c>
       <c r="D70" t="s">
-        <v>218</v>
+        <v>117</v>
       </c>
       <c r="E70" t="s">
-        <v>211</v>
+        <v>129</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>68</v>
+        <v>187</v>
       </c>
       <c r="H70" t="s">
-        <v>120</v>
+        <v>214</v>
       </c>
       <c r="I70" t="s">
-        <v>139</v>
+        <v>209</v>
       </c>
     </row>
     <row r="71" spans="1:9">
       <c r="A71" s="1" t="s">
-        <v>69</v>
+        <v>2</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>26</v>
+        <v>192</v>
       </c>
       <c r="D71" t="s">
-        <v>118</v>
+        <v>218</v>
       </c>
       <c r="E71" t="s">
-        <v>141</v>
+        <v>211</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="H71" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I71" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
     </row>
     <row r="72" spans="1:9">
       <c r="A72" s="1" t="s">
-        <v>4</v>
+        <v>69</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="D72" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E72" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="H72" t="s">
         <v>121</v>
@@ -2999,79 +3048,79 @@
     </row>
     <row r="73" spans="1:9">
       <c r="A73" s="1" t="s">
-        <v>77</v>
+        <v>4</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>187</v>
+        <v>43</v>
       </c>
       <c r="D73" t="s">
-        <v>214</v>
+        <v>119</v>
       </c>
       <c r="E73" t="s">
-        <v>209</v>
+        <v>136</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>159</v>
+        <v>51</v>
       </c>
       <c r="H73" t="s">
-        <v>163</v>
+        <v>121</v>
       </c>
       <c r="I73" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="74" spans="1:9">
       <c r="A74" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>68</v>
+        <v>187</v>
       </c>
       <c r="D74" t="s">
-        <v>120</v>
+        <v>214</v>
       </c>
       <c r="E74" t="s">
-        <v>139</v>
+        <v>209</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>161</v>
+        <v>237</v>
       </c>
       <c r="H74" t="s">
-        <v>165</v>
+        <v>240</v>
       </c>
       <c r="I74" t="s">
-        <v>166</v>
+        <v>135</v>
       </c>
     </row>
     <row r="75" spans="1:9">
       <c r="A75" s="1" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="D75" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E75" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>21</v>
+        <v>159</v>
       </c>
       <c r="H75" t="s">
-        <v>122</v>
+        <v>163</v>
       </c>
       <c r="I75" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
     </row>
     <row r="76" spans="1:9">
       <c r="A76" s="1" t="s">
-        <v>173</v>
+        <v>33</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="D76" t="s">
         <v>121</v>
@@ -3080,217 +3129,217 @@
         <v>134</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>64</v>
+        <v>161</v>
       </c>
       <c r="H76" t="s">
-        <v>123</v>
+        <v>165</v>
       </c>
       <c r="I76" t="s">
-        <v>147</v>
+        <v>166</v>
       </c>
     </row>
     <row r="77" spans="1:9">
       <c r="A77" s="1" t="s">
-        <v>18</v>
+        <v>173</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>159</v>
+        <v>51</v>
       </c>
       <c r="D77" t="s">
-        <v>163</v>
+        <v>121</v>
       </c>
       <c r="E77" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>195</v>
+        <v>21</v>
       </c>
       <c r="H77" t="s">
-        <v>221</v>
+        <v>122</v>
       </c>
       <c r="I77" t="s">
-        <v>222</v>
+        <v>146</v>
       </c>
     </row>
     <row r="78" spans="1:9">
       <c r="A78" s="1" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>161</v>
+        <v>237</v>
       </c>
       <c r="D78" t="s">
-        <v>165</v>
+        <v>240</v>
       </c>
       <c r="E78" t="s">
-        <v>166</v>
+        <v>135</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>160</v>
+        <v>64</v>
       </c>
       <c r="H78" t="s">
-        <v>164</v>
+        <v>123</v>
       </c>
       <c r="I78" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
     </row>
     <row r="79" spans="1:9">
       <c r="A79" s="1" t="s">
-        <v>39</v>
+        <v>1</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>21</v>
+        <v>159</v>
       </c>
       <c r="D79" t="s">
-        <v>122</v>
+        <v>163</v>
       </c>
       <c r="E79" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>29</v>
+        <v>195</v>
       </c>
       <c r="H79" t="s">
-        <v>124</v>
+        <v>221</v>
       </c>
       <c r="I79" t="s">
-        <v>131</v>
+        <v>222</v>
       </c>
     </row>
     <row r="80" spans="1:9">
       <c r="A80" s="1" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>64</v>
+        <v>161</v>
       </c>
       <c r="D80" t="s">
-        <v>123</v>
+        <v>165</v>
       </c>
       <c r="E80" t="s">
-        <v>147</v>
+        <v>166</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>52</v>
+        <v>160</v>
       </c>
       <c r="H80" t="s">
-        <v>125</v>
+        <v>164</v>
       </c>
       <c r="I80" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="81" spans="1:9">
       <c r="A81" s="1" t="s">
-        <v>6</v>
+        <v>65</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>195</v>
+        <v>21</v>
       </c>
       <c r="D81" t="s">
-        <v>221</v>
+        <v>122</v>
       </c>
       <c r="E81" t="s">
-        <v>222</v>
+        <v>146</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>194</v>
+        <v>29</v>
       </c>
       <c r="H81" t="s">
-        <v>220</v>
+        <v>124</v>
       </c>
       <c r="I81" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="82" spans="1:9">
       <c r="A82" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>160</v>
+        <v>64</v>
       </c>
       <c r="D82" t="s">
-        <v>164</v>
+        <v>123</v>
       </c>
       <c r="E82" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="H82" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I82" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
     </row>
     <row r="83" spans="1:9">
       <c r="A83" s="1" t="s">
-        <v>192</v>
+        <v>17</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>29</v>
+        <v>195</v>
       </c>
       <c r="D83" t="s">
-        <v>124</v>
+        <v>221</v>
       </c>
       <c r="E83" t="s">
-        <v>131</v>
+        <v>222</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>3</v>
+        <v>194</v>
       </c>
       <c r="H83" t="s">
-        <v>127</v>
+        <v>220</v>
       </c>
       <c r="I83" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
     </row>
     <row r="84" spans="1:9">
       <c r="A84" s="1" t="s">
-        <v>9</v>
+        <v>192</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>52</v>
+        <v>160</v>
       </c>
       <c r="D84" t="s">
-        <v>125</v>
+        <v>164</v>
       </c>
       <c r="E84" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>203</v>
+        <v>28</v>
       </c>
       <c r="H84" t="s">
-        <v>230</v>
+        <v>126</v>
       </c>
       <c r="I84" t="s">
-        <v>231</v>
+        <v>131</v>
       </c>
     </row>
     <row r="85" spans="1:9">
       <c r="A85" s="1" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>194</v>
+        <v>29</v>
       </c>
       <c r="D85" t="s">
-        <v>220</v>
+        <v>124</v>
       </c>
       <c r="E85" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="H85" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I85" t="s">
         <v>129</v>
@@ -3298,68 +3347,68 @@
     </row>
     <row r="86" spans="1:9">
       <c r="A86" s="1" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="D86" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E86" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>188</v>
+        <v>203</v>
       </c>
       <c r="H86" t="s">
-        <v>215</v>
+        <v>230</v>
       </c>
       <c r="I86" t="s">
-        <v>209</v>
+        <v>231</v>
       </c>
     </row>
     <row r="87" spans="1:9">
       <c r="A87" s="1" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>3</v>
+        <v>194</v>
       </c>
       <c r="D87" t="s">
-        <v>127</v>
+        <v>220</v>
       </c>
       <c r="E87" t="s">
+        <v>136</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H87" t="s">
+        <v>128</v>
+      </c>
+      <c r="I87" t="s">
         <v>129</v>
-      </c>
-      <c r="G87" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H87" t="s">
-        <v>235</v>
-      </c>
-      <c r="I87" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="88" spans="1:9">
       <c r="A88" s="1" t="s">
-        <v>187</v>
+        <v>43</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>203</v>
+        <v>28</v>
       </c>
       <c r="D88" t="s">
-        <v>230</v>
+        <v>126</v>
       </c>
       <c r="E88" t="s">
-        <v>231</v>
+        <v>131</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H88" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I88" t="s">
         <v>209</v>
@@ -3367,64 +3416,82 @@
     </row>
     <row r="89" spans="1:9">
       <c r="A89" s="1" t="s">
-        <v>68</v>
+        <v>187</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="D89" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E89" t="s">
         <v>129</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="H89" t="s">
-        <v>224</v>
+        <v>235</v>
       </c>
       <c r="I89" t="s">
-        <v>225</v>
+        <v>142</v>
       </c>
     </row>
     <row r="90" spans="1:9">
       <c r="A90" s="1" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>188</v>
+        <v>203</v>
       </c>
       <c r="D90" t="s">
-        <v>215</v>
+        <v>230</v>
       </c>
       <c r="E90" t="s">
+        <v>231</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H90" t="s">
+        <v>216</v>
+      </c>
+      <c r="I90" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="91" spans="1:9">
       <c r="A91" s="1" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>207</v>
+        <v>55</v>
       </c>
       <c r="D91" t="s">
-        <v>235</v>
+        <v>128</v>
       </c>
       <c r="E91" t="s">
-        <v>142</v>
+        <v>129</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="H91" t="s">
+        <v>224</v>
+      </c>
+      <c r="I91" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="92" spans="1:9">
       <c r="A92" s="1" t="s">
-        <v>159</v>
+        <v>51</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D92" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E92" t="s">
         <v>209</v>
@@ -3432,125 +3499,153 @@
     </row>
     <row r="93" spans="1:9">
       <c r="A93" s="1" t="s">
-        <v>161</v>
+        <v>237</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="D93" t="s">
-        <v>224</v>
+        <v>235</v>
       </c>
       <c r="E93" t="s">
-        <v>225</v>
+        <v>142</v>
       </c>
     </row>
     <row r="94" spans="1:9">
       <c r="A94" s="1" t="s">
-        <v>35</v>
+        <v>159</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D94" t="s">
+        <v>216</v>
+      </c>
+      <c r="E94" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="95" spans="1:9">
       <c r="A95" s="1" t="s">
-        <v>21</v>
+        <v>161</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D95" t="s">
+        <v>224</v>
+      </c>
+      <c r="E95" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="96" spans="1:9">
       <c r="A96" s="1" t="s">
-        <v>64</v>
+        <v>35</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" s="1" t="s">
-        <v>195</v>
+        <v>21</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" s="1" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" s="1" t="s">
-        <v>160</v>
+        <v>195</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" s="1" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" s="1" t="s">
-        <v>29</v>
+        <v>160</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" s="1" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" s="1" t="s">
-        <v>197</v>
+        <v>29</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" s="1" t="s">
-        <v>194</v>
+        <v>52</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105" s="1" t="s">
-        <v>28</v>
+        <v>197</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106" s="1" t="s">
-        <v>3</v>
+        <v>194</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107" s="1" t="s">
-        <v>203</v>
+        <v>28</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108" s="1" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109" s="1" t="s">
-        <v>188</v>
+        <v>203</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110" s="1" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" s="1" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" s="1" t="s">
-        <v>63</v>
+        <v>11</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" s="1" t="s">
-        <v>189</v>
+        <v>207</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116" s="1" t="s">
         <v>198</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="G9:I89">
+  <sortState ref="G9:I91">
     <sortCondition ref="G9"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3565,10 +3660,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:M85"/>
+  <dimension ref="B4:M88"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView showRuler="0" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="C90" sqref="C90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3830,7 +3925,7 @@
         <v>142</v>
       </c>
       <c r="J17" s="10">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K17" s="10"/>
       <c r="L17" s="10"/>
@@ -4140,30 +4235,30 @@
     </row>
     <row r="33" spans="2:13">
       <c r="B33" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>161</v>
+        <v>238</v>
       </c>
       <c r="D33" t="s">
-        <v>165</v>
+        <v>239</v>
       </c>
       <c r="I33" s="13" t="s">
         <v>236</v>
       </c>
       <c r="J33" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="2:13">
       <c r="B34" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>67</v>
+        <v>161</v>
       </c>
       <c r="D34" t="s">
-        <v>93</v>
+        <v>165</v>
       </c>
     </row>
     <row r="35" spans="2:13">
@@ -4171,17 +4266,17 @@
         <v>139</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D35" t="s">
-        <v>120</v>
+        <v>93</v>
       </c>
       <c r="I35" s="12" t="s">
         <v>177</v>
       </c>
       <c r="J35" s="10">
         <f>SUM(J8:J33)</f>
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="K35" s="10"/>
       <c r="L35" s="10"/>
@@ -4192,13 +4287,13 @@
     </row>
     <row r="36" spans="2:13">
       <c r="B36" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="D36" t="s">
-        <v>86</v>
+        <v>120</v>
       </c>
     </row>
     <row r="37" spans="2:13">
@@ -4206,10 +4301,10 @@
         <v>136</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>75</v>
+        <v>38</v>
       </c>
       <c r="D37" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" spans="2:13">
@@ -4217,10 +4312,10 @@
         <v>136</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>49</v>
+        <v>75</v>
       </c>
       <c r="D38" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="39" spans="2:13">
@@ -4228,10 +4323,10 @@
         <v>136</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="D39" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="40" spans="2:13">
@@ -4239,10 +4334,10 @@
         <v>136</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D40" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="41" spans="2:13">
@@ -4250,10 +4345,10 @@
         <v>136</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D41" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
     </row>
     <row r="42" spans="2:13">
@@ -4261,10 +4356,10 @@
         <v>136</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>160</v>
+        <v>43</v>
       </c>
       <c r="D42" t="s">
-        <v>164</v>
+        <v>119</v>
       </c>
     </row>
     <row r="43" spans="2:13">
@@ -4272,21 +4367,21 @@
         <v>136</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>194</v>
+        <v>160</v>
       </c>
       <c r="D43" t="s">
-        <v>220</v>
+        <v>164</v>
       </c>
     </row>
     <row r="44" spans="2:13">
       <c r="B44" t="s">
-        <v>211</v>
+        <v>136</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D44" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="45" spans="2:13">
@@ -4294,10 +4389,10 @@
         <v>211</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D45" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="46" spans="2:13">
@@ -4305,21 +4400,21 @@
         <v>211</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D46" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="47" spans="2:13">
       <c r="B47" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>78</v>
+        <v>192</v>
       </c>
       <c r="D47" t="s">
-        <v>92</v>
+        <v>218</v>
       </c>
     </row>
     <row r="48" spans="2:13">
@@ -4327,10 +4422,10 @@
         <v>210</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>199</v>
+        <v>78</v>
       </c>
       <c r="D48" t="s">
-        <v>226</v>
+        <v>92</v>
       </c>
     </row>
     <row r="49" spans="2:4">
@@ -4338,10 +4433,10 @@
         <v>210</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="D49" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="50" spans="2:4">
@@ -4349,10 +4444,10 @@
         <v>210</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D50" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="51" spans="2:4">
@@ -4360,32 +4455,32 @@
         <v>210</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>73</v>
+        <v>200</v>
       </c>
       <c r="D51" t="s">
-        <v>84</v>
+        <v>227</v>
       </c>
     </row>
     <row r="52" spans="2:4">
       <c r="B52" t="s">
-        <v>146</v>
+        <v>210</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>21</v>
+        <v>73</v>
       </c>
       <c r="D52" t="s">
-        <v>122</v>
+        <v>84</v>
       </c>
     </row>
     <row r="53" spans="2:4">
       <c r="B53" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>181</v>
+        <v>21</v>
       </c>
       <c r="D53" t="s">
-        <v>182</v>
+        <v>122</v>
       </c>
     </row>
     <row r="54" spans="2:4">
@@ -4393,10 +4488,10 @@
         <v>145</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="D54" t="s">
-        <v>228</v>
+        <v>182</v>
       </c>
     </row>
     <row r="55" spans="2:4">
@@ -4404,21 +4499,21 @@
         <v>145</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>39</v>
+        <v>201</v>
       </c>
       <c r="D55" t="s">
-        <v>115</v>
+        <v>228</v>
       </c>
     </row>
     <row r="56" spans="2:4">
       <c r="B56" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="D56" t="s">
-        <v>149</v>
+        <v>115</v>
       </c>
     </row>
     <row r="57" spans="2:4">
@@ -4426,10 +4521,10 @@
         <v>129</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>76</v>
+        <v>7</v>
       </c>
       <c r="D57" t="s">
-        <v>87</v>
+        <v>149</v>
       </c>
     </row>
     <row r="58" spans="2:4">
@@ -4437,10 +4532,10 @@
         <v>129</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>5</v>
+        <v>76</v>
       </c>
       <c r="D58" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
     </row>
     <row r="59" spans="2:4">
@@ -4448,10 +4543,10 @@
         <v>129</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D59" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
     </row>
     <row r="60" spans="2:4">
@@ -4459,10 +4554,10 @@
         <v>129</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>77</v>
+        <v>4</v>
       </c>
       <c r="D60" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="61" spans="2:4">
@@ -4470,10 +4565,10 @@
         <v>129</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="D61" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="62" spans="2:4">
@@ -4481,10 +4576,10 @@
         <v>129</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="D62" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="63" spans="2:4">
@@ -4492,32 +4587,32 @@
         <v>129</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="D63" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="64" spans="2:4">
       <c r="B64" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="D64" t="s">
-        <v>103</v>
+        <v>128</v>
       </c>
     </row>
     <row r="65" spans="2:4">
       <c r="B65" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D65" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
     </row>
     <row r="66" spans="2:4">
@@ -4525,10 +4620,10 @@
         <v>134</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>202</v>
+        <v>50</v>
       </c>
       <c r="D66" t="s">
-        <v>229</v>
+        <v>83</v>
       </c>
     </row>
     <row r="67" spans="2:4">
@@ -4536,10 +4631,10 @@
         <v>134</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>157</v>
+        <v>202</v>
       </c>
       <c r="D67" t="s">
-        <v>162</v>
+        <v>229</v>
       </c>
     </row>
     <row r="68" spans="2:4">
@@ -4547,10 +4642,10 @@
         <v>134</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>16</v>
+        <v>157</v>
       </c>
       <c r="D68" t="s">
-        <v>121</v>
+        <v>162</v>
       </c>
     </row>
     <row r="69" spans="2:4">
@@ -4558,7 +4653,7 @@
         <v>134</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="D69" t="s">
         <v>121</v>
@@ -4566,13 +4661,13 @@
     </row>
     <row r="70" spans="2:4">
       <c r="B70" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="D70" t="s">
-        <v>81</v>
+        <v>121</v>
       </c>
     </row>
     <row r="71" spans="2:4">
@@ -4580,21 +4675,21 @@
         <v>132</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>159</v>
+        <v>74</v>
       </c>
       <c r="D71" t="s">
-        <v>163</v>
+        <v>81</v>
       </c>
     </row>
     <row r="72" spans="2:4">
       <c r="B72" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>61</v>
+        <v>159</v>
       </c>
       <c r="D72" t="s">
-        <v>148</v>
+        <v>163</v>
       </c>
     </row>
     <row r="73" spans="2:4">
@@ -4602,10 +4697,10 @@
         <v>141</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D73" t="s">
-        <v>95</v>
+        <v>148</v>
       </c>
     </row>
     <row r="74" spans="2:4">
@@ -4613,10 +4708,10 @@
         <v>141</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="D74" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="75" spans="2:4">
@@ -4624,7 +4719,7 @@
         <v>141</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="D75" t="s">
         <v>104</v>
@@ -4635,10 +4730,10 @@
         <v>141</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="D76" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="77" spans="2:4">
@@ -4646,10 +4741,10 @@
         <v>141</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D77" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="78" spans="2:4">
@@ -4657,10 +4752,10 @@
         <v>141</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="D78" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="79" spans="2:4">
@@ -4668,10 +4763,10 @@
         <v>141</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="D79" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="80" spans="2:4">
@@ -4679,70 +4774,96 @@
         <v>141</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D80" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="81" spans="2:4">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="81" spans="2:7">
       <c r="B81" t="s">
         <v>141</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="D81" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="82" spans="2:4">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7">
       <c r="B82" t="s">
         <v>141</v>
       </c>
       <c r="C82" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D82" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="83" spans="2:7">
+      <c r="B83" t="s">
+        <v>141</v>
+      </c>
+      <c r="C83" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D82" t="s">
+      <c r="D83" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="83" spans="2:4">
-      <c r="B83" t="s">
+    <row r="84" spans="2:7">
+      <c r="B84" t="s">
         <v>151</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="C84" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D83" t="s">
+      <c r="D84" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="84" spans="2:4">
-      <c r="B84" t="s">
+    <row r="85" spans="2:7">
+      <c r="B85" t="s">
         <v>222</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="C85" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="D84" t="s">
+      <c r="D85" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="85" spans="2:4">
-      <c r="B85" t="s">
+    <row r="86" spans="2:7">
+      <c r="B86" t="s">
         <v>135</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="C86" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D86" t="s">
         <v>114</v>
       </c>
     </row>
+    <row r="87" spans="2:7">
+      <c r="B87" t="s">
+        <v>135</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D87" t="s">
+        <v>240</v>
+      </c>
+      <c r="G87" s="1"/>
+    </row>
+    <row r="88" spans="2:7">
+      <c r="G88" s="1"/>
+    </row>
   </sheetData>
-  <sortState ref="I43:K65">
-    <sortCondition ref="K43"/>
+  <sortState ref="B4:D87">
+    <sortCondition ref="B4"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Added users to the Excel file Removed unused references to Filestore Updated description of maintenance pipeline method
</commit_message>
<xml_diff>
--- a/Janelia Workstation User List.xlsx
+++ b/Janelia Workstation User List.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="929" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="249">
   <si>
     <t>bukowinskip</t>
   </si>
@@ -758,6 +758,15 @@
   </si>
   <si>
     <t>riddiford</t>
+  </si>
+  <si>
+    <t>hustons</t>
+  </si>
+  <si>
+    <t>Stephen Huston</t>
+  </si>
+  <si>
+    <t>Huston</t>
   </si>
 </sst>
 </file>
@@ -873,12 +882,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="126">
+  <cellStyleXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1022,7 +1033,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="126">
+  <cellStyles count="128">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -1088,6 +1099,7 @@
     <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
@@ -1148,6 +1160,7 @@
     <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1477,10 +1490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I117"/>
+  <dimension ref="A1:I118"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G93" sqref="G93:I93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3531,6 +3544,15 @@
       <c r="E93" t="s">
         <v>142</v>
       </c>
+      <c r="G93" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="H93" t="s">
+        <v>247</v>
+      </c>
+      <c r="I93" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="94" spans="1:9">
       <c r="A94" s="1" t="s">
@@ -3574,82 +3596,91 @@
         <v>244</v>
       </c>
     </row>
-    <row r="97" spans="1:1">
+    <row r="97" spans="1:5">
       <c r="A97" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="98" spans="1:1">
+      <c r="C97" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D97" t="s">
+        <v>247</v>
+      </c>
+      <c r="E97" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
       <c r="A98" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="99" spans="1:1">
+    <row r="99" spans="1:5">
       <c r="A99" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="100" spans="1:1">
+    <row r="100" spans="1:5">
       <c r="A100" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="101" spans="1:1">
+    <row r="101" spans="1:5">
       <c r="A101" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="102" spans="1:1">
+    <row r="102" spans="1:5">
       <c r="A102" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="103" spans="1:1">
+    <row r="103" spans="1:5">
       <c r="A103" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="104" spans="1:1">
+    <row r="104" spans="1:5">
       <c r="A104" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="105" spans="1:1">
+    <row r="105" spans="1:5">
       <c r="A105" s="1" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="106" spans="1:1">
+    <row r="106" spans="1:5">
       <c r="A106" s="1" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="107" spans="1:1">
+    <row r="107" spans="1:5">
       <c r="A107" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="108" spans="1:1">
+    <row r="108" spans="1:5">
       <c r="A108" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="1:1">
+    <row r="109" spans="1:5">
       <c r="A109" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="110" spans="1:1">
+    <row r="110" spans="1:5">
       <c r="A110" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="111" spans="1:1">
+    <row r="111" spans="1:5">
       <c r="A111" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="112" spans="1:1">
+    <row r="112" spans="1:5">
       <c r="A112" s="1" t="s">
         <v>11</v>
       </c>
@@ -3677,6 +3708,11 @@
     <row r="117" spans="1:1">
       <c r="A117" s="1" t="s">
         <v>242</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" s="1" t="s">
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -3695,10 +3731,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:M88"/>
+  <dimension ref="B4:M89"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="K37" sqref="K37"/>
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4296,7 +4332,7 @@
         <v>165</v>
       </c>
       <c r="I34" s="13" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="J34" s="14">
         <v>1</v>
@@ -4312,17 +4348,10 @@
       <c r="D35" t="s">
         <v>93</v>
       </c>
-      <c r="I35" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="J35" s="10">
-        <f>SUM(J8:J34)</f>
-        <v>85</v>
-      </c>
-      <c r="K35" s="10"/>
-      <c r="L35" s="10"/>
-      <c r="M35" s="11">
-        <f>SUM(M8:M33)</f>
+      <c r="I35" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="J35" s="14">
         <v>1</v>
       </c>
     </row>
@@ -4336,6 +4365,19 @@
       <c r="D36" t="s">
         <v>120</v>
       </c>
+      <c r="I36" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="J36" s="10">
+        <f>SUM(J8:J35)</f>
+        <v>86</v>
+      </c>
+      <c r="K36" s="10"/>
+      <c r="L36" s="10"/>
+      <c r="M36" s="11">
+        <f>SUM(M8:M33)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="37" spans="2:13">
       <c r="B37" t="s">
@@ -4910,6 +4952,17 @@
         <v>243</v>
       </c>
       <c r="G88" s="1"/>
+    </row>
+    <row r="89" spans="2:7">
+      <c r="B89" t="s">
+        <v>248</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D89" t="s">
+        <v>247</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="B4:D87">

</xml_diff>

<commit_message>
Added Zhengchang Lei to the user file
</commit_message>
<xml_diff>
--- a/Janelia Workstation User List.xlsx
+++ b/Janelia Workstation User List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="37360" windowHeight="23560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="37360" windowHeight="23560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Raw User Data From LDAP" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="960" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="255">
   <si>
     <t>bukowinskip</t>
   </si>
@@ -779,6 +779,12 @@
   </si>
   <si>
     <t>Nan Chen</t>
+  </si>
+  <si>
+    <t>leiz</t>
+  </si>
+  <si>
+    <t>Zhengchang Lei</t>
   </si>
 </sst>
 </file>
@@ -901,12 +907,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="144">
+  <cellStyleXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1069,7 +1077,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="144">
+  <cellStyles count="146">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -1144,6 +1152,7 @@
     <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
@@ -1213,6 +1222,7 @@
     <cellStyle name="Hyperlink" xfId="138" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="140" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="142" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="144" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1542,10 +1552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I120"/>
+  <dimension ref="A1:I121"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView showRuler="0" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="H96" sqref="G96:I96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3665,6 +3675,15 @@
       <c r="E96" t="s">
         <v>244</v>
       </c>
+      <c r="G96" t="s">
+        <v>253</v>
+      </c>
+      <c r="H96" t="s">
+        <v>254</v>
+      </c>
+      <c r="I96" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="1" t="s">
@@ -3712,6 +3731,15 @@
       <c r="A100" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="C100" t="s">
+        <v>253</v>
+      </c>
+      <c r="D100" t="s">
+        <v>254</v>
+      </c>
+      <c r="E100" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="1" t="s">
@@ -3811,6 +3839,11 @@
     <row r="120" spans="1:1">
       <c r="A120" s="1" t="s">
         <v>251</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1">
+      <c r="A121" s="1" t="s">
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -3829,10 +3862,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:M91"/>
+  <dimension ref="B4:M92"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5084,6 +5117,17 @@
         <v>240</v>
       </c>
     </row>
+    <row r="92" spans="2:7">
+      <c r="B92" t="s">
+        <v>211</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="D92" t="s">
+        <v>254</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="B4:D91">
     <sortCondition ref="B4:B91"/>

</xml_diff>

<commit_message>
Bumped version numbers for release.  h5j correction service.
</commit_message>
<xml_diff>
--- a/Janelia Workstation User List.xlsx
+++ b/Janelia Workstation User List.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1235" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1247" uniqueCount="312">
   <si>
     <t>bukowinskip</t>
   </si>
@@ -920,6 +920,42 @@
   </si>
   <si>
     <t>Ito</t>
+  </si>
+  <si>
+    <t>bermang</t>
+  </si>
+  <si>
+    <t>Gordon Berman</t>
+  </si>
+  <si>
+    <t>ribeiroi</t>
+  </si>
+  <si>
+    <t>Ines Ribeiro</t>
+  </si>
+  <si>
+    <t>wangf12</t>
+  </si>
+  <si>
+    <t>Fei Wang</t>
+  </si>
+  <si>
+    <t>arthurb</t>
+  </si>
+  <si>
+    <t>otsunah</t>
+  </si>
+  <si>
+    <t>Ben Arthur</t>
+  </si>
+  <si>
+    <t>Hideo Otsuna</t>
+  </si>
+  <si>
+    <t>Celia Beron</t>
+  </si>
+  <si>
+    <t>beronc</t>
   </si>
 </sst>
 </file>
@@ -932,7 +968,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="136"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1027,7 +1063,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="205">
+  <cellStyleXfs count="206">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1233,6 +1269,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1261,7 +1298,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="204"/>
   </cellXfs>
-  <cellStyles count="205">
+  <cellStyles count="206">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -1370,6 +1407,7 @@
     <cellStyle name="Followed Hyperlink" xfId="199" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="201" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="203" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="205" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
@@ -1795,9 +1833,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K144"/>
+  <dimension ref="A1:K151"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A146" sqref="A146:A151"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -4681,6 +4721,54 @@
     <row r="144" spans="1:7">
       <c r="A144" s="1" t="s">
         <v>190</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2">
+      <c r="A146" t="s">
+        <v>300</v>
+      </c>
+      <c r="B146" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2">
+      <c r="A147" t="s">
+        <v>302</v>
+      </c>
+      <c r="B147" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2">
+      <c r="A148" t="s">
+        <v>304</v>
+      </c>
+      <c r="B148" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2">
+      <c r="A149" t="s">
+        <v>306</v>
+      </c>
+      <c r="B149" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2">
+      <c r="A150" t="s">
+        <v>307</v>
+      </c>
+      <c r="B150" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2">
+      <c r="A151" t="s">
+        <v>311</v>
+      </c>
+      <c r="B151" t="s">
+        <v>310</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
User list update.  New pipeline error email account.  IntelliJ build directory cleanup for NetBeans
</commit_message>
<xml_diff>
--- a/Janelia Workstation User List.xlsx
+++ b/Janelia Workstation User List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="360" windowWidth="35700" windowHeight="22620" tabRatio="500"/>
+    <workbookView xWindow="440" yWindow="360" windowWidth="35700" windowHeight="22620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Raw User Data From LDAP" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1344" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1346" uniqueCount="327">
   <si>
     <t>bukowinskip</t>
   </si>
@@ -1896,10 +1896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K159"/>
+  <dimension ref="A1:K161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A115" sqref="A115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5040,6 +5040,16 @@
     <row r="159" spans="1:2">
       <c r="A159" t="s">
         <v>324</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2">
+      <c r="A160" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1">
+      <c r="A161" t="s">
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Joda Time into IntelliJ module dependency User list update Project points to Java 8
</commit_message>
<xml_diff>
--- a/Janelia Workstation User List.xlsx
+++ b/Janelia Workstation User List.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1346" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1371" uniqueCount="334">
   <si>
     <t>bukowinskip</t>
   </si>
@@ -1001,19 +1001,39 @@
   </si>
   <si>
     <t>Johan Winnubst</t>
+  </si>
+  <si>
+    <t>collinsa</t>
+  </si>
+  <si>
+    <t>frechters</t>
+  </si>
+  <si>
+    <t>Shahar Frechter</t>
+  </si>
+  <si>
+    <t>Amanda Collins</t>
+  </si>
+  <si>
+    <t>goinac</t>
+  </si>
+  <si>
+    <t>ohashi</t>
+  </si>
+  <si>
+    <t>Takako Ohashi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1043,6 +1063,13 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1108,7 +1135,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="212">
+  <cellStyleXfs count="215">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1321,8 +1348,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1354,8 +1384,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="212">
+  <cellStyles count="215">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -1471,6 +1505,9 @@
     <cellStyle name="Followed Hyperlink" xfId="209" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="211" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="213" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
@@ -1896,10 +1933,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K161"/>
+  <dimension ref="A1:K165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A115" sqref="A115"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1918,7 +1955,7 @@
         <v>152</v>
       </c>
       <c r="B1" s="4">
-        <v>40765</v>
+        <v>40806</v>
       </c>
       <c r="D1" s="6"/>
       <c r="E1" s="5" t="s">
@@ -4858,7 +4895,15 @@
       <c r="E132" t="s">
         <v>201</v>
       </c>
-      <c r="G132" s="1"/>
+      <c r="G132" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="H132" t="s">
+        <v>330</v>
+      </c>
+      <c r="I132" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="133" spans="1:9">
       <c r="A133" s="1" t="s">
@@ -4873,7 +4918,15 @@
       <c r="E133" t="s">
         <v>138</v>
       </c>
-      <c r="G133" s="1"/>
+      <c r="G133" t="s">
+        <v>328</v>
+      </c>
+      <c r="H133" t="s">
+        <v>329</v>
+      </c>
+      <c r="I133" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="134" spans="1:9">
       <c r="A134" s="1" t="s">
@@ -4888,6 +4941,15 @@
       <c r="E134" t="s">
         <v>201</v>
       </c>
+      <c r="G134" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="H134" t="s">
+        <v>333</v>
+      </c>
+      <c r="I134" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="135" spans="1:9">
       <c r="A135" s="1" t="s">
@@ -4935,16 +4997,43 @@
       <c r="A138" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="C138" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D138" t="s">
+        <v>330</v>
+      </c>
+      <c r="E138" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="139" spans="1:9">
       <c r="A139" s="1" t="s">
         <v>180</v>
       </c>
+      <c r="C139" t="s">
+        <v>328</v>
+      </c>
+      <c r="D139" t="s">
+        <v>329</v>
+      </c>
+      <c r="E139" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="140" spans="1:9">
       <c r="A140" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="C140" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="D140" t="s">
+        <v>333</v>
+      </c>
+      <c r="E140" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="141" spans="1:9">
       <c r="A141" s="1" t="s">
@@ -5050,6 +5139,26 @@
     <row r="161" spans="1:1">
       <c r="A161" t="s">
         <v>300</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1">
+      <c r="A162" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1">
+      <c r="A163" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1">
+      <c r="A164" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1">
+      <c r="A165" t="s">
+        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -5068,11 +5177,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:M131"/>
+  <dimension ref="B4:M132"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I47" sqref="I47"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -5513,7 +5620,7 @@
         <v>202</v>
       </c>
       <c r="J26" s="8">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K26" s="15"/>
       <c r="L26" s="11"/>
@@ -5790,7 +5897,7 @@
       </c>
       <c r="J40" s="8">
         <f>SUM(J8:J39)</f>
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K40" s="15"/>
     </row>
@@ -6180,33 +6287,33 @@
       </c>
     </row>
     <row r="76" spans="2:4">
-      <c r="B76" s="1" t="s">
+      <c r="B76" s="23" t="s">
+        <v>332</v>
+      </c>
+      <c r="C76" s="24" t="s">
+        <v>333</v>
+      </c>
+      <c r="D76" s="24" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4">
+      <c r="B77" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C77" t="s">
         <v>243</v>
-      </c>
-      <c r="D76" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="77" spans="2:4">
-      <c r="B77" t="s">
-        <v>271</v>
-      </c>
-      <c r="C77" t="s">
-        <v>142</v>
       </c>
       <c r="D77" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="78" spans="2:4">
-      <c r="B78" s="1" t="s">
-        <v>19</v>
+      <c r="B78" t="s">
+        <v>271</v>
       </c>
       <c r="C78" t="s">
-        <v>119</v>
+        <v>142</v>
       </c>
       <c r="D78" t="s">
         <v>142</v>
@@ -6214,21 +6321,21 @@
     </row>
     <row r="79" spans="2:4">
       <c r="B79" s="1" t="s">
-        <v>173</v>
+        <v>19</v>
       </c>
       <c r="C79" t="s">
-        <v>174</v>
+        <v>119</v>
       </c>
       <c r="D79" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="80" spans="2:4">
       <c r="B80" s="1" t="s">
-        <v>193</v>
+        <v>173</v>
       </c>
       <c r="C80" t="s">
-        <v>220</v>
+        <v>174</v>
       </c>
       <c r="D80" t="s">
         <v>141</v>
@@ -6236,21 +6343,21 @@
     </row>
     <row r="81" spans="2:7">
       <c r="B81" s="1" t="s">
-        <v>36</v>
+        <v>193</v>
       </c>
       <c r="C81" t="s">
-        <v>112</v>
+        <v>220</v>
       </c>
       <c r="D81" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="82" spans="2:7">
-      <c r="B82" t="s">
-        <v>276</v>
+      <c r="B82" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="C82" t="s">
-        <v>286</v>
+        <v>112</v>
       </c>
       <c r="D82" t="s">
         <v>141</v>
@@ -6258,32 +6365,32 @@
     </row>
     <row r="83" spans="2:7">
       <c r="B83" t="s">
+        <v>276</v>
+      </c>
+      <c r="C83" t="s">
+        <v>286</v>
+      </c>
+      <c r="D83" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="84" spans="2:7">
+      <c r="B84" t="s">
         <v>234</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C84" t="s">
         <v>235</v>
       </c>
-      <c r="D83" t="s">
+      <c r="D84" t="s">
         <v>236</v>
-      </c>
-    </row>
-    <row r="84" spans="2:7">
-      <c r="B84" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C84" t="s">
-        <v>145</v>
-      </c>
-      <c r="D84" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="85" spans="2:7">
       <c r="B85" s="1" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="C85" t="s">
-        <v>84</v>
+        <v>145</v>
       </c>
       <c r="D85" t="s">
         <v>126</v>
@@ -6291,10 +6398,10 @@
     </row>
     <row r="86" spans="2:7">
       <c r="B86" s="1" t="s">
-        <v>5</v>
+        <v>73</v>
       </c>
       <c r="C86" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="D86" t="s">
         <v>126</v>
@@ -6302,10 +6409,10 @@
     </row>
     <row r="87" spans="2:7">
       <c r="B87" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C87" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="D87" t="s">
         <v>126</v>
@@ -6314,10 +6421,10 @@
     </row>
     <row r="88" spans="2:7">
       <c r="B88" s="1" t="s">
-        <v>74</v>
+        <v>4</v>
       </c>
       <c r="C88" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D88" t="s">
         <v>126</v>
@@ -6326,10 +6433,10 @@
     </row>
     <row r="89" spans="2:7">
       <c r="B89" s="1" t="s">
-        <v>15</v>
+        <v>74</v>
       </c>
       <c r="C89" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D89" t="s">
         <v>126</v>
@@ -6337,10 +6444,10 @@
     </row>
     <row r="90" spans="2:7">
       <c r="B90" s="1" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="C90" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="D90" t="s">
         <v>126</v>
@@ -6348,10 +6455,10 @@
     </row>
     <row r="91" spans="2:7">
       <c r="B91" s="1" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="C91" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D91" t="s">
         <v>126</v>
@@ -6359,32 +6466,32 @@
     </row>
     <row r="92" spans="2:7">
       <c r="B92" s="1" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="C92" t="s">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="D92" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
     </row>
     <row r="93" spans="2:7">
       <c r="B93" s="1" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="C93" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="D93" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
     </row>
     <row r="94" spans="2:7">
       <c r="B94" s="1" t="s">
-        <v>194</v>
+        <v>47</v>
       </c>
       <c r="C94" t="s">
-        <v>221</v>
+        <v>80</v>
       </c>
       <c r="D94" t="s">
         <v>131</v>
@@ -6392,10 +6499,10 @@
     </row>
     <row r="95" spans="2:7">
       <c r="B95" s="1" t="s">
-        <v>153</v>
+        <v>194</v>
       </c>
       <c r="C95" t="s">
-        <v>158</v>
+        <v>221</v>
       </c>
       <c r="D95" t="s">
         <v>131</v>
@@ -6403,10 +6510,10 @@
     </row>
     <row r="96" spans="2:7">
       <c r="B96" s="1" t="s">
-        <v>14</v>
+        <v>153</v>
       </c>
       <c r="C96" t="s">
-        <v>118</v>
+        <v>158</v>
       </c>
       <c r="D96" t="s">
         <v>131</v>
@@ -6414,7 +6521,7 @@
     </row>
     <row r="97" spans="2:4">
       <c r="B97" s="1" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C97" t="s">
         <v>118</v>
@@ -6425,43 +6532,43 @@
     </row>
     <row r="98" spans="2:4">
       <c r="B98" s="1" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="C98" t="s">
-        <v>78</v>
+        <v>118</v>
       </c>
       <c r="D98" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="99" spans="2:4">
       <c r="B99" s="1" t="s">
-        <v>155</v>
+        <v>71</v>
       </c>
       <c r="C99" t="s">
-        <v>159</v>
+        <v>78</v>
       </c>
       <c r="D99" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="100" spans="2:4">
-      <c r="B100" t="s">
-        <v>290</v>
+      <c r="B100" s="1" t="s">
+        <v>155</v>
       </c>
       <c r="C100" t="s">
-        <v>294</v>
+        <v>159</v>
       </c>
       <c r="D100" t="s">
-        <v>295</v>
+        <v>129</v>
       </c>
     </row>
     <row r="101" spans="2:4">
       <c r="B101" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C101" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D101" t="s">
         <v>295</v>
@@ -6469,32 +6576,32 @@
     </row>
     <row r="102" spans="2:4">
       <c r="B102" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C102" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="D102" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="103" spans="2:4">
-      <c r="B103" s="1" t="s">
-        <v>58</v>
+      <c r="B103" t="s">
+        <v>292</v>
       </c>
       <c r="C103" t="s">
-        <v>144</v>
+        <v>296</v>
       </c>
       <c r="D103" t="s">
-        <v>137</v>
+        <v>295</v>
       </c>
     </row>
     <row r="104" spans="2:4">
       <c r="B104" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C104" t="s">
-        <v>92</v>
+        <v>144</v>
       </c>
       <c r="D104" t="s">
         <v>137</v>
@@ -6502,10 +6609,10 @@
     </row>
     <row r="105" spans="2:4">
       <c r="B105" s="1" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="C105" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="D105" t="s">
         <v>137</v>
@@ -6513,7 +6620,7 @@
     </row>
     <row r="106" spans="2:4">
       <c r="B106" s="1" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="C106" t="s">
         <v>101</v>
@@ -6524,10 +6631,10 @@
     </row>
     <row r="107" spans="2:4">
       <c r="B107" s="1" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="C107" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D107" t="s">
         <v>137</v>
@@ -6535,10 +6642,10 @@
     </row>
     <row r="108" spans="2:4">
       <c r="B108" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C108" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D108" t="s">
         <v>137</v>
@@ -6546,10 +6653,10 @@
     </row>
     <row r="109" spans="2:4">
       <c r="B109" s="1" t="s">
-        <v>18</v>
+        <v>56</v>
       </c>
       <c r="C109" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D109" t="s">
         <v>137</v>
@@ -6557,10 +6664,10 @@
     </row>
     <row r="110" spans="2:4">
       <c r="B110" s="1" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
       <c r="C110" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D110" t="s">
         <v>137</v>
@@ -6568,10 +6675,10 @@
     </row>
     <row r="111" spans="2:4">
       <c r="B111" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C111" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="D111" t="s">
         <v>137</v>
@@ -6579,10 +6686,10 @@
     </row>
     <row r="112" spans="2:4">
       <c r="B112" s="1" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="C112" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D112" t="s">
         <v>137</v>
@@ -6590,10 +6697,10 @@
     </row>
     <row r="113" spans="2:4">
       <c r="B113" s="1" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="C113" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="D113" t="s">
         <v>137</v>
@@ -6601,32 +6708,32 @@
     </row>
     <row r="114" spans="2:4">
       <c r="B114" s="1" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="C114" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="D114" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="115" spans="2:4">
       <c r="B115" s="1" t="s">
-        <v>63</v>
+        <v>24</v>
       </c>
       <c r="C115" t="s">
-        <v>79</v>
+        <v>146</v>
       </c>
       <c r="D115" t="s">
-        <v>130</v>
+        <v>147</v>
       </c>
     </row>
     <row r="116" spans="2:4">
       <c r="B116" s="1" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="C116" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D116" t="s">
         <v>130</v>
@@ -6634,10 +6741,10 @@
     </row>
     <row r="117" spans="2:4">
       <c r="B117" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C117" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D117" t="s">
         <v>130</v>
@@ -6645,32 +6752,32 @@
     </row>
     <row r="118" spans="2:4">
       <c r="B118" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C118" t="s">
+        <v>88</v>
+      </c>
+      <c r="D118" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="119" spans="2:4">
+      <c r="B119" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="C118" t="s">
+      <c r="C119" t="s">
         <v>213</v>
       </c>
-      <c r="D118" t="s">
+      <c r="D119" t="s">
         <v>214</v>
-      </c>
-    </row>
-    <row r="119" spans="2:4">
-      <c r="B119" t="s">
-        <v>273</v>
-      </c>
-      <c r="C119" t="s">
-        <v>283</v>
-      </c>
-      <c r="D119" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="120" spans="2:4">
       <c r="B120" t="s">
-        <v>252</v>
+        <v>273</v>
       </c>
       <c r="C120" t="s">
-        <v>253</v>
+        <v>283</v>
       </c>
       <c r="D120" t="s">
         <v>132</v>
@@ -6678,10 +6785,10 @@
     </row>
     <row r="121" spans="2:4">
       <c r="B121" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="C121" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="D121" t="s">
         <v>132</v>
@@ -6689,10 +6796,10 @@
     </row>
     <row r="122" spans="2:4">
       <c r="B122" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="C122" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="D122" t="s">
         <v>132</v>
@@ -6700,10 +6807,10 @@
     </row>
     <row r="123" spans="2:4">
       <c r="B123" t="s">
-        <v>274</v>
+        <v>258</v>
       </c>
       <c r="C123" t="s">
-        <v>284</v>
+        <v>259</v>
       </c>
       <c r="D123" t="s">
         <v>132</v>
@@ -6711,21 +6818,21 @@
     </row>
     <row r="124" spans="2:4">
       <c r="B124" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="C124" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="D124" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="125" spans="2:4">
-      <c r="B125" s="1" t="s">
-        <v>16</v>
+      <c r="B125" t="s">
+        <v>272</v>
       </c>
       <c r="C125" t="s">
-        <v>111</v>
+        <v>282</v>
       </c>
       <c r="D125" t="s">
         <v>132</v>
@@ -6733,21 +6840,21 @@
     </row>
     <row r="126" spans="2:4">
       <c r="B126" s="1" t="s">
-        <v>229</v>
+        <v>16</v>
       </c>
       <c r="C126" t="s">
-        <v>232</v>
+        <v>111</v>
       </c>
       <c r="D126" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="127" spans="2:4">
-      <c r="B127" t="s">
-        <v>300</v>
+      <c r="B127" s="1" t="s">
+        <v>229</v>
       </c>
       <c r="C127" t="s">
-        <v>301</v>
+        <v>232</v>
       </c>
       <c r="D127" t="s">
         <v>132</v>
@@ -6755,10 +6862,10 @@
     </row>
     <row r="128" spans="2:4">
       <c r="B128" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="C128" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
       <c r="D128" t="s">
         <v>132</v>
@@ -6766,34 +6873,45 @@
     </row>
     <row r="129" spans="2:4">
       <c r="B129" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C129" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="D129" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="130" spans="2:4">
-      <c r="B130" s="1" t="s">
-        <v>322</v>
+      <c r="B130" t="s">
+        <v>314</v>
       </c>
       <c r="C130" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="D130" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="131" spans="2:4">
       <c r="B131" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="C131" t="s">
+        <v>325</v>
+      </c>
+      <c r="D131" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="132" spans="2:4">
+      <c r="B132" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="C131" t="s">
+      <c r="C132" t="s">
         <v>326</v>
       </c>
-      <c r="D131" t="s">
+      <c r="D132" t="s">
         <v>202</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Corey Fisher to the user list
</commit_message>
<xml_diff>
--- a/Janelia Workstation User List.xlsx
+++ b/Janelia Workstation User List.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1371" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1381" uniqueCount="337">
   <si>
     <t>bukowinskip</t>
   </si>
@@ -1022,6 +1022,15 @@
   </si>
   <si>
     <t>Takako Ohashi</t>
+  </si>
+  <si>
+    <t>fischerc</t>
+  </si>
+  <si>
+    <t>fisherc</t>
+  </si>
+  <si>
+    <t>Corey Fischer</t>
   </si>
 </sst>
 </file>
@@ -1135,7 +1144,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="215">
+  <cellStyleXfs count="217">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1341,6 +1350,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1389,7 +1400,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="215">
+  <cellStyles count="217">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -1508,6 +1519,8 @@
     <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="213" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="215" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
@@ -1933,10 +1946,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K165"/>
+  <dimension ref="A1:K166"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A142" sqref="A142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4964,6 +4977,15 @@
       <c r="E135" t="s">
         <v>217</v>
       </c>
+      <c r="G135" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="H135" t="s">
+        <v>336</v>
+      </c>
+      <c r="I135" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="136" spans="1:9">
       <c r="A136" s="1" t="s">
@@ -5039,6 +5061,15 @@
       <c r="A141" s="1" t="s">
         <v>199</v>
       </c>
+      <c r="C141" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="D141" t="s">
+        <v>336</v>
+      </c>
+      <c r="E141" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="142" spans="1:9">
       <c r="A142" s="1" t="s">
@@ -5159,6 +5190,11 @@
     <row r="165" spans="1:1">
       <c r="A165" t="s">
         <v>332</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1">
+      <c r="A166" t="s">
+        <v>334</v>
       </c>
     </row>
   </sheetData>
@@ -5177,9 +5213,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:M132"/>
+  <dimension ref="B4:M133"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8:J38"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -5280,7 +5318,7 @@
         <v>217</v>
       </c>
       <c r="J9" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K9" s="15"/>
       <c r="L9" s="11"/>
@@ -5897,7 +5935,7 @@
       </c>
       <c r="J40" s="8">
         <f>SUM(J8:J39)</f>
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="K40" s="15"/>
     </row>
@@ -6913,6 +6951,17 @@
       </c>
       <c r="D132" t="s">
         <v>202</v>
+      </c>
+    </row>
+    <row r="133" spans="2:4">
+      <c r="B133" s="23" t="s">
+        <v>335</v>
+      </c>
+      <c r="C133" s="24" t="s">
+        <v>336</v>
+      </c>
+      <c r="D133" s="24" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bump version numbers.  Fixed project.properties.  Update center in.  New users
</commit_message>
<xml_diff>
--- a/Janelia Workstation User List.xlsx
+++ b/Janelia Workstation User List.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1428" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1484" uniqueCount="363">
   <si>
     <t>bukowinskip</t>
   </si>
@@ -1061,6 +1061,54 @@
   </si>
   <si>
     <t>Saalfeld</t>
+  </si>
+  <si>
+    <t>cavallaroa</t>
+  </si>
+  <si>
+    <t>sharpb</t>
+  </si>
+  <si>
+    <t>gonzalezg</t>
+  </si>
+  <si>
+    <t>coffmans</t>
+  </si>
+  <si>
+    <t>mercerm</t>
+  </si>
+  <si>
+    <t>zhengg</t>
+  </si>
+  <si>
+    <t>dangt</t>
+  </si>
+  <si>
+    <t>lavertyt</t>
+  </si>
+  <si>
+    <t>Amanda Cavallaro</t>
+  </si>
+  <si>
+    <t>Brandi Sharp</t>
+  </si>
+  <si>
+    <t>Guillermo Gonzales</t>
+  </si>
+  <si>
+    <t>Scarlett Coffman</t>
+  </si>
+  <si>
+    <t>Monti Mercer</t>
+  </si>
+  <si>
+    <t>Grace Zheng</t>
+  </si>
+  <si>
+    <t>Tam Dang</t>
+  </si>
+  <si>
+    <t>Todd Laverty</t>
   </si>
 </sst>
 </file>
@@ -1073,6 +1121,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1174,7 +1223,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="225">
+  <cellStyleXfs count="246">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1380,6 +1429,27 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1438,7 +1508,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="225">
+  <cellStyles count="246">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -1567,6 +1637,27 @@
     <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="223" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="225" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="227" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="229" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="231" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="233" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="235" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="237" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="239" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="241" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="243" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="245" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
@@ -1992,10 +2083,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K170"/>
+  <dimension ref="A1:K178"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A137" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C146" sqref="C146:C153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5213,41 +5304,113 @@
       <c r="A146" t="s">
         <v>246</v>
       </c>
+      <c r="C146" t="s">
+        <v>347</v>
+      </c>
+      <c r="D146" t="s">
+        <v>355</v>
+      </c>
+      <c r="E146" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="147" spans="1:5">
       <c r="A147" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="C147" t="s">
+        <v>348</v>
+      </c>
+      <c r="D147" t="s">
+        <v>356</v>
+      </c>
+      <c r="E147" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="148" spans="1:5">
       <c r="A148" s="1" t="s">
         <v>61</v>
       </c>
+      <c r="C148" t="s">
+        <v>349</v>
+      </c>
+      <c r="D148" t="s">
+        <v>357</v>
+      </c>
+      <c r="E148" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="149" spans="1:5">
       <c r="A149" s="1" t="s">
         <v>187</v>
       </c>
+      <c r="C149" t="s">
+        <v>350</v>
+      </c>
+      <c r="D149" t="s">
+        <v>358</v>
+      </c>
+      <c r="E149" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="150" spans="1:5">
       <c r="A150" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="C150" t="s">
+        <v>351</v>
+      </c>
+      <c r="D150" t="s">
+        <v>359</v>
+      </c>
+      <c r="E150" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="151" spans="1:5">
       <c r="A151" s="1" t="s">
         <v>156</v>
       </c>
+      <c r="C151" t="s">
+        <v>352</v>
+      </c>
+      <c r="D151" t="s">
+        <v>360</v>
+      </c>
+      <c r="E151" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="152" spans="1:5">
       <c r="A152" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="C152" t="s">
+        <v>353</v>
+      </c>
+      <c r="D152" t="s">
+        <v>361</v>
+      </c>
+      <c r="E152" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="153" spans="1:5">
       <c r="A153" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="C153" t="s">
+        <v>354</v>
+      </c>
+      <c r="D153" t="s">
+        <v>362</v>
+      </c>
+      <c r="E153" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="154" spans="1:5">
       <c r="A154" s="1" t="s">
@@ -5333,6 +5496,46 @@
     <row r="170" spans="1:1">
       <c r="A170" s="1" t="s">
         <v>190</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1">
+      <c r="A171" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1">
+      <c r="A172" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1">
+      <c r="A173" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1">
+      <c r="A174" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1">
+      <c r="A175" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1">
+      <c r="A176" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1">
+      <c r="A177" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1">
+      <c r="A178" t="s">
+        <v>354</v>
       </c>
     </row>
   </sheetData>
@@ -5351,10 +5554,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:M144"/>
+  <dimension ref="B4:M147"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:D147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5903,14 +6106,14 @@
       <c r="M31" s="13"/>
     </row>
     <row r="32" spans="2:13">
-      <c r="B32" s="1" t="s">
-        <v>195</v>
+      <c r="B32" t="s">
+        <v>347</v>
       </c>
       <c r="C32" t="s">
-        <v>222</v>
+        <v>355</v>
       </c>
       <c r="D32" t="s">
-        <v>223</v>
+        <v>136</v>
       </c>
       <c r="I32" s="15" t="s">
         <v>139</v>
@@ -5923,14 +6126,14 @@
       <c r="M32" s="13"/>
     </row>
     <row r="33" spans="2:13">
-      <c r="B33" s="1" t="s">
-        <v>43</v>
+      <c r="B33" t="s">
+        <v>348</v>
       </c>
       <c r="C33" t="s">
-        <v>106</v>
+        <v>356</v>
       </c>
       <c r="D33" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="I33" s="15" t="s">
         <v>131</v>
@@ -5943,14 +6146,14 @@
       <c r="M33" s="13"/>
     </row>
     <row r="34" spans="2:13">
-      <c r="B34" s="1" t="s">
-        <v>230</v>
+      <c r="B34" t="s">
+        <v>349</v>
       </c>
       <c r="C34" t="s">
-        <v>231</v>
+        <v>357</v>
       </c>
       <c r="D34" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="I34" s="15" t="s">
         <v>129</v>
@@ -5963,14 +6166,14 @@
       <c r="M34" s="13"/>
     </row>
     <row r="35" spans="2:13">
-      <c r="B35" s="1" t="s">
-        <v>44</v>
+      <c r="B35" t="s">
+        <v>350</v>
       </c>
       <c r="C35" t="s">
-        <v>93</v>
+        <v>358</v>
       </c>
       <c r="D35" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="I35" s="15" t="s">
         <v>295</v>
@@ -5983,14 +6186,14 @@
       <c r="M35" s="13"/>
     </row>
     <row r="36" spans="2:13">
-      <c r="B36" s="1" t="s">
-        <v>59</v>
+      <c r="B36" t="s">
+        <v>351</v>
       </c>
       <c r="C36" t="s">
-        <v>96</v>
+        <v>359</v>
       </c>
       <c r="D36" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="I36" s="15" t="s">
         <v>137</v>
@@ -6003,14 +6206,14 @@
       <c r="M36" s="13"/>
     </row>
     <row r="37" spans="2:13">
-      <c r="B37" s="1" t="s">
-        <v>55</v>
+      <c r="B37" t="s">
+        <v>352</v>
       </c>
       <c r="C37" t="s">
-        <v>97</v>
+        <v>360</v>
       </c>
       <c r="D37" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="I37" s="16" t="s">
         <v>130</v>
@@ -6023,14 +6226,14 @@
       <c r="M37" s="13"/>
     </row>
     <row r="38" spans="2:13">
-      <c r="B38" s="1" t="s">
-        <v>68</v>
+      <c r="B38" t="s">
+        <v>353</v>
       </c>
       <c r="C38" t="s">
-        <v>98</v>
+        <v>361</v>
       </c>
       <c r="D38" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="I38" s="16" t="s">
         <v>214</v>
@@ -6043,14 +6246,14 @@
       <c r="M38" s="13"/>
     </row>
     <row r="39" spans="2:13">
-      <c r="B39" s="1" t="s">
-        <v>196</v>
+      <c r="B39" t="s">
+        <v>354</v>
       </c>
       <c r="C39" t="s">
-        <v>224</v>
+        <v>362</v>
       </c>
       <c r="D39" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="I39" s="19" t="s">
         <v>228</v>
@@ -6064,13 +6267,13 @@
     </row>
     <row r="40" spans="2:13">
       <c r="B40" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C40" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="D40" t="s">
-        <v>138</v>
+        <v>223</v>
       </c>
       <c r="I40" s="16"/>
       <c r="J40" s="11"/>
@@ -6078,10 +6281,10 @@
     </row>
     <row r="41" spans="2:13">
       <c r="B41" s="1" t="s">
-        <v>197</v>
+        <v>43</v>
       </c>
       <c r="C41" t="s">
-        <v>225</v>
+        <v>106</v>
       </c>
       <c r="D41" t="s">
         <v>138</v>
@@ -6097,32 +6300,32 @@
     </row>
     <row r="42" spans="2:13">
       <c r="B42" s="1" t="s">
-        <v>2</v>
+        <v>230</v>
       </c>
       <c r="C42" t="s">
-        <v>107</v>
+        <v>231</v>
       </c>
       <c r="D42" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="43" spans="2:13">
-      <c r="B43" t="s">
-        <v>269</v>
+      <c r="B43" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="C43" t="s">
-        <v>280</v>
+        <v>93</v>
       </c>
       <c r="D43" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="44" spans="2:13">
-      <c r="B44" t="s">
-        <v>250</v>
+      <c r="B44" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="C44" t="s">
-        <v>251</v>
+        <v>96</v>
       </c>
       <c r="D44" t="s">
         <v>138</v>
@@ -6130,826 +6333,826 @@
     </row>
     <row r="45" spans="2:13">
       <c r="B45" s="1" t="s">
-        <v>199</v>
+        <v>55</v>
       </c>
       <c r="C45" t="s">
-        <v>227</v>
+        <v>97</v>
       </c>
       <c r="D45" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="46" spans="2:13">
-      <c r="B46" t="s">
-        <v>316</v>
+      <c r="B46" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="C46" t="s">
-        <v>317</v>
+        <v>98</v>
       </c>
       <c r="D46" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="47" spans="2:13">
-      <c r="B47" s="24" t="s">
-        <v>344</v>
-      </c>
-      <c r="C47" s="24" t="s">
-        <v>345</v>
-      </c>
-      <c r="D47" s="24" t="s">
+      <c r="B47" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C47" t="s">
+        <v>224</v>
+      </c>
+      <c r="D47" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="48" spans="2:13">
       <c r="B48" s="1" t="s">
-        <v>157</v>
+        <v>198</v>
       </c>
       <c r="C48" t="s">
-        <v>161</v>
+        <v>226</v>
       </c>
       <c r="D48" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
     </row>
     <row r="49" spans="2:4">
       <c r="B49" s="1" t="s">
-        <v>64</v>
+        <v>197</v>
       </c>
       <c r="C49" t="s">
-        <v>90</v>
+        <v>225</v>
       </c>
       <c r="D49" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="50" spans="2:4">
-      <c r="B50" t="s">
-        <v>240</v>
+      <c r="B50" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="C50" t="s">
-        <v>241</v>
+        <v>107</v>
       </c>
       <c r="D50" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="51" spans="2:4">
-      <c r="B51" s="1" t="s">
-        <v>65</v>
+      <c r="B51" t="s">
+        <v>269</v>
       </c>
       <c r="C51" t="s">
-        <v>117</v>
+        <v>280</v>
       </c>
       <c r="D51" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="52" spans="2:4">
-      <c r="B52" s="1" t="s">
-        <v>262</v>
+      <c r="B52" t="s">
+        <v>250</v>
       </c>
       <c r="C52" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="D52" t="s">
-        <v>266</v>
+        <v>138</v>
       </c>
     </row>
     <row r="53" spans="2:4">
       <c r="B53" s="1" t="s">
-        <v>237</v>
+        <v>199</v>
       </c>
       <c r="C53" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="D53" t="s">
-        <v>239</v>
+        <v>138</v>
       </c>
     </row>
     <row r="54" spans="2:4">
       <c r="B54" t="s">
-        <v>279</v>
+        <v>316</v>
       </c>
       <c r="C54" t="s">
-        <v>289</v>
+        <v>317</v>
       </c>
       <c r="D54" t="s">
-        <v>299</v>
+        <v>138</v>
       </c>
     </row>
     <row r="55" spans="2:4">
-      <c r="B55" t="s">
-        <v>278</v>
-      </c>
-      <c r="C55" t="s">
-        <v>288</v>
-      </c>
-      <c r="D55" t="s">
-        <v>299</v>
+      <c r="B55" s="24" t="s">
+        <v>344</v>
+      </c>
+      <c r="C55" s="24" t="s">
+        <v>345</v>
+      </c>
+      <c r="D55" s="24" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="56" spans="2:4">
-      <c r="B56" t="s">
-        <v>277</v>
+      <c r="B56" s="1" t="s">
+        <v>157</v>
       </c>
       <c r="C56" t="s">
-        <v>287</v>
+        <v>161</v>
       </c>
       <c r="D56" t="s">
-        <v>299</v>
+        <v>162</v>
       </c>
     </row>
     <row r="57" spans="2:4">
       <c r="B57" s="1" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="C57" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="D57" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="58" spans="2:4">
-      <c r="B58" s="1" t="s">
-        <v>72</v>
+      <c r="B58" t="s">
+        <v>240</v>
       </c>
       <c r="C58" t="s">
-        <v>86</v>
+        <v>241</v>
       </c>
       <c r="D58" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="59" spans="2:4">
       <c r="B59" s="1" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="C59" t="s">
-        <v>87</v>
+        <v>117</v>
       </c>
       <c r="D59" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="60" spans="2:4">
       <c r="B60" s="1" t="s">
-        <v>34</v>
+        <v>262</v>
       </c>
       <c r="C60" t="s">
-        <v>94</v>
+        <v>263</v>
       </c>
       <c r="D60" t="s">
-        <v>133</v>
+        <v>266</v>
       </c>
     </row>
     <row r="61" spans="2:4">
       <c r="B61" s="1" t="s">
-        <v>37</v>
+        <v>237</v>
       </c>
       <c r="C61" t="s">
-        <v>99</v>
+        <v>238</v>
       </c>
       <c r="D61" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4">
+      <c r="B62" t="s">
+        <v>279</v>
+      </c>
+      <c r="C62" t="s">
+        <v>289</v>
+      </c>
+      <c r="D62" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4">
+      <c r="B63" t="s">
+        <v>278</v>
+      </c>
+      <c r="C63" t="s">
+        <v>288</v>
+      </c>
+      <c r="D63" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4">
+      <c r="B64" t="s">
+        <v>277</v>
+      </c>
+      <c r="C64" t="s">
+        <v>287</v>
+      </c>
+      <c r="D64" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4">
+      <c r="B65" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C65" t="s">
+        <v>83</v>
+      </c>
+      <c r="D65" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="62" spans="2:4">
-      <c r="B62" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C62" t="s">
-        <v>116</v>
-      </c>
-      <c r="D62" t="s">
+    <row r="66" spans="2:4">
+      <c r="B66" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C66" t="s">
+        <v>86</v>
+      </c>
+      <c r="D66" t="s">
         <v>133</v>
-      </c>
-    </row>
-    <row r="63" spans="2:4">
-      <c r="B63" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C63" t="s">
-        <v>160</v>
-      </c>
-      <c r="D63" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="64" spans="2:4">
-      <c r="B64" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="C64" t="s">
-        <v>212</v>
-      </c>
-      <c r="D64" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="65" spans="2:4">
-      <c r="B65" s="24" t="s">
-        <v>337</v>
-      </c>
-      <c r="C65" s="24" t="s">
-        <v>338</v>
-      </c>
-      <c r="D65" s="24" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="66" spans="2:4">
-      <c r="B66" t="s">
-        <v>309</v>
-      </c>
-      <c r="C66" t="s">
-        <v>308</v>
-      </c>
-      <c r="D66" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="67" spans="2:4">
       <c r="B67" s="1" t="s">
-        <v>185</v>
+        <v>46</v>
       </c>
       <c r="C67" t="s">
-        <v>211</v>
+        <v>87</v>
       </c>
       <c r="D67" t="s">
-        <v>203</v>
+        <v>133</v>
       </c>
     </row>
     <row r="68" spans="2:4">
       <c r="B68" s="1" t="s">
-        <v>183</v>
+        <v>34</v>
       </c>
       <c r="C68" t="s">
-        <v>209</v>
+        <v>94</v>
       </c>
       <c r="D68" t="s">
-        <v>203</v>
+        <v>133</v>
       </c>
     </row>
     <row r="69" spans="2:4">
-      <c r="B69" t="s">
-        <v>244</v>
+      <c r="B69" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="C69" t="s">
-        <v>245</v>
+        <v>99</v>
       </c>
       <c r="D69" t="s">
-        <v>203</v>
+        <v>133</v>
       </c>
     </row>
     <row r="70" spans="2:4">
       <c r="B70" s="1" t="s">
-        <v>184</v>
+        <v>40</v>
       </c>
       <c r="C70" t="s">
-        <v>210</v>
+        <v>116</v>
       </c>
       <c r="D70" t="s">
-        <v>203</v>
+        <v>133</v>
       </c>
     </row>
     <row r="71" spans="2:4">
-      <c r="B71" t="s">
-        <v>267</v>
+      <c r="B71" s="1" t="s">
+        <v>156</v>
       </c>
       <c r="C71" t="s">
-        <v>268</v>
+        <v>160</v>
       </c>
       <c r="D71" t="s">
-        <v>202</v>
+        <v>133</v>
       </c>
     </row>
     <row r="72" spans="2:4">
       <c r="B72" s="1" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C72" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="D72" t="s">
-        <v>202</v>
+        <v>133</v>
       </c>
     </row>
     <row r="73" spans="2:4">
-      <c r="B73" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C73" t="s">
-        <v>81</v>
-      </c>
-      <c r="D73" t="s">
-        <v>202</v>
+      <c r="B73" s="24" t="s">
+        <v>337</v>
+      </c>
+      <c r="C73" s="24" t="s">
+        <v>338</v>
+      </c>
+      <c r="D73" s="24" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="74" spans="2:4">
-      <c r="B74" s="1" t="s">
-        <v>188</v>
+      <c r="B74" t="s">
+        <v>309</v>
       </c>
       <c r="C74" t="s">
-        <v>215</v>
+        <v>308</v>
       </c>
       <c r="D74" t="s">
-        <v>202</v>
+        <v>313</v>
       </c>
     </row>
     <row r="75" spans="2:4">
       <c r="B75" s="1" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="C75" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="D75" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="76" spans="2:4">
       <c r="B76" s="1" t="s">
-        <v>75</v>
+        <v>183</v>
       </c>
       <c r="C76" t="s">
-        <v>89</v>
+        <v>209</v>
       </c>
       <c r="D76" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="77" spans="2:4">
       <c r="B77" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C77" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D77" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="78" spans="2:4">
-      <c r="B78" t="s">
-        <v>320</v>
+      <c r="B78" s="1" t="s">
+        <v>184</v>
       </c>
       <c r="C78" t="s">
-        <v>321</v>
+        <v>210</v>
       </c>
       <c r="D78" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="79" spans="2:4">
-      <c r="B79" s="23" t="s">
-        <v>332</v>
-      </c>
-      <c r="C79" s="24" t="s">
-        <v>333</v>
-      </c>
-      <c r="D79" s="24" t="s">
+      <c r="B79" t="s">
+        <v>267</v>
+      </c>
+      <c r="C79" t="s">
+        <v>268</v>
+      </c>
+      <c r="D79" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="80" spans="2:4">
       <c r="B80" s="1" t="s">
-        <v>324</v>
+        <v>191</v>
       </c>
       <c r="C80" t="s">
-        <v>326</v>
+        <v>218</v>
       </c>
       <c r="D80" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="81" spans="2:7">
-      <c r="B81" s="23" t="s">
-        <v>327</v>
-      </c>
-      <c r="C81" s="24" t="s">
-        <v>330</v>
-      </c>
-      <c r="D81" s="24" t="s">
+      <c r="B81" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C81" t="s">
+        <v>81</v>
+      </c>
+      <c r="D81" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="82" spans="2:7">
       <c r="B82" s="1" t="s">
-        <v>242</v>
+        <v>188</v>
       </c>
       <c r="C82" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
       <c r="D82" t="s">
-        <v>142</v>
+        <v>202</v>
       </c>
     </row>
     <row r="83" spans="2:7">
-      <c r="B83" t="s">
-        <v>271</v>
+      <c r="B83" s="1" t="s">
+        <v>192</v>
       </c>
       <c r="C83" t="s">
-        <v>142</v>
+        <v>219</v>
       </c>
       <c r="D83" t="s">
-        <v>142</v>
+        <v>202</v>
       </c>
     </row>
     <row r="84" spans="2:7">
       <c r="B84" s="1" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="C84" t="s">
-        <v>119</v>
+        <v>89</v>
       </c>
       <c r="D84" t="s">
-        <v>142</v>
+        <v>202</v>
       </c>
     </row>
     <row r="85" spans="2:7">
-      <c r="B85" s="24" t="s">
-        <v>339</v>
-      </c>
-      <c r="C85" s="24" t="s">
-        <v>340</v>
-      </c>
-      <c r="D85" s="24" t="s">
-        <v>142</v>
+      <c r="B85" t="s">
+        <v>246</v>
+      </c>
+      <c r="C85" t="s">
+        <v>247</v>
+      </c>
+      <c r="D85" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="86" spans="2:7">
-      <c r="B86" s="1" t="s">
-        <v>173</v>
+      <c r="B86" t="s">
+        <v>320</v>
       </c>
       <c r="C86" t="s">
-        <v>174</v>
+        <v>321</v>
       </c>
       <c r="D86" t="s">
-        <v>141</v>
+        <v>202</v>
       </c>
     </row>
     <row r="87" spans="2:7">
-      <c r="B87" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="C87" t="s">
-        <v>220</v>
-      </c>
-      <c r="D87" t="s">
-        <v>141</v>
+      <c r="B87" s="23" t="s">
+        <v>332</v>
+      </c>
+      <c r="C87" s="24" t="s">
+        <v>333</v>
+      </c>
+      <c r="D87" s="24" t="s">
+        <v>202</v>
       </c>
       <c r="G87" s="1"/>
     </row>
     <row r="88" spans="2:7">
       <c r="B88" s="1" t="s">
-        <v>36</v>
+        <v>324</v>
       </c>
       <c r="C88" t="s">
-        <v>112</v>
+        <v>326</v>
       </c>
       <c r="D88" t="s">
-        <v>141</v>
+        <v>202</v>
       </c>
       <c r="G88" s="1"/>
     </row>
     <row r="89" spans="2:7">
-      <c r="B89" t="s">
-        <v>276</v>
-      </c>
-      <c r="C89" t="s">
-        <v>286</v>
-      </c>
-      <c r="D89" t="s">
-        <v>141</v>
+      <c r="B89" s="23" t="s">
+        <v>327</v>
+      </c>
+      <c r="C89" s="24" t="s">
+        <v>330</v>
+      </c>
+      <c r="D89" s="24" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="90" spans="2:7">
-      <c r="B90" t="s">
-        <v>234</v>
+      <c r="B90" s="1" t="s">
+        <v>242</v>
       </c>
       <c r="C90" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="D90" t="s">
-        <v>236</v>
+        <v>142</v>
       </c>
     </row>
     <row r="91" spans="2:7">
-      <c r="B91" s="1" t="s">
-        <v>7</v>
+      <c r="B91" t="s">
+        <v>271</v>
       </c>
       <c r="C91" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D91" t="s">
-        <v>126</v>
+        <v>142</v>
       </c>
     </row>
     <row r="92" spans="2:7">
       <c r="B92" s="1" t="s">
-        <v>73</v>
+        <v>19</v>
       </c>
       <c r="C92" t="s">
-        <v>84</v>
+        <v>119</v>
       </c>
       <c r="D92" t="s">
-        <v>126</v>
+        <v>142</v>
       </c>
     </row>
     <row r="93" spans="2:7">
-      <c r="B93" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C93" t="s">
-        <v>95</v>
-      </c>
-      <c r="D93" t="s">
-        <v>126</v>
+      <c r="B93" s="24" t="s">
+        <v>339</v>
+      </c>
+      <c r="C93" s="24" t="s">
+        <v>340</v>
+      </c>
+      <c r="D93" s="24" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="94" spans="2:7">
       <c r="B94" s="1" t="s">
-        <v>4</v>
+        <v>173</v>
       </c>
       <c r="C94" t="s">
-        <v>109</v>
+        <v>174</v>
       </c>
       <c r="D94" t="s">
-        <v>126</v>
+        <v>141</v>
       </c>
     </row>
     <row r="95" spans="2:7">
       <c r="B95" s="1" t="s">
-        <v>74</v>
+        <v>193</v>
       </c>
       <c r="C95" t="s">
-        <v>110</v>
+        <v>220</v>
       </c>
       <c r="D95" t="s">
-        <v>126</v>
+        <v>141</v>
       </c>
     </row>
     <row r="96" spans="2:7">
       <c r="B96" s="1" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="C96" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D96" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="97" spans="2:4">
+      <c r="B97" t="s">
+        <v>276</v>
+      </c>
+      <c r="C97" t="s">
+        <v>286</v>
+      </c>
+      <c r="D97" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="98" spans="2:4">
+      <c r="B98" t="s">
+        <v>234</v>
+      </c>
+      <c r="C98" t="s">
+        <v>235</v>
+      </c>
+      <c r="D98" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="99" spans="2:4">
+      <c r="B99" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C99" t="s">
+        <v>145</v>
+      </c>
+      <c r="D99" t="s">
         <v>126</v>
-      </c>
-    </row>
-    <row r="97" spans="2:4">
-      <c r="B97" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C97" t="s">
-        <v>124</v>
-      </c>
-      <c r="D97" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="98" spans="2:4">
-      <c r="B98" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C98" t="s">
-        <v>125</v>
-      </c>
-      <c r="D98" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="99" spans="2:4">
-      <c r="B99" s="24" t="s">
-        <v>341</v>
-      </c>
-      <c r="C99" s="24" t="s">
-        <v>342</v>
-      </c>
-      <c r="D99" s="24" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="100" spans="2:4">
       <c r="B100" s="1" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="C100" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="D100" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
     </row>
     <row r="101" spans="2:4">
       <c r="B101" s="1" t="s">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="C101" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="D101" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="102" spans="2:4">
       <c r="B102" s="1" t="s">
-        <v>194</v>
+        <v>4</v>
       </c>
       <c r="C102" t="s">
-        <v>221</v>
+        <v>109</v>
       </c>
       <c r="D102" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="103" spans="2:4">
       <c r="B103" s="1" t="s">
-        <v>153</v>
+        <v>74</v>
       </c>
       <c r="C103" t="s">
-        <v>158</v>
+        <v>110</v>
       </c>
       <c r="D103" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="104" spans="2:4">
       <c r="B104" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C104" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D104" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="105" spans="2:4">
       <c r="B105" s="1" t="s">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="C105" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="D105" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="106" spans="2:4">
       <c r="B106" s="1" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="C106" t="s">
-        <v>78</v>
+        <v>125</v>
       </c>
       <c r="D106" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="107" spans="2:4">
-      <c r="B107" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C107" t="s">
-        <v>159</v>
-      </c>
-      <c r="D107" t="s">
-        <v>129</v>
+      <c r="B107" s="24" t="s">
+        <v>341</v>
+      </c>
+      <c r="C107" s="24" t="s">
+        <v>342</v>
+      </c>
+      <c r="D107" s="24" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="108" spans="2:4">
-      <c r="B108" t="s">
-        <v>290</v>
+      <c r="B108" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="C108" t="s">
-        <v>294</v>
+        <v>100</v>
       </c>
       <c r="D108" t="s">
-        <v>295</v>
+        <v>139</v>
       </c>
     </row>
     <row r="109" spans="2:4">
-      <c r="B109" t="s">
-        <v>291</v>
+      <c r="B109" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="C109" t="s">
-        <v>298</v>
+        <v>80</v>
       </c>
       <c r="D109" t="s">
-        <v>295</v>
+        <v>131</v>
       </c>
     </row>
     <row r="110" spans="2:4">
-      <c r="B110" t="s">
-        <v>292</v>
+      <c r="B110" s="1" t="s">
+        <v>194</v>
       </c>
       <c r="C110" t="s">
-        <v>296</v>
+        <v>221</v>
       </c>
       <c r="D110" t="s">
-        <v>295</v>
+        <v>131</v>
       </c>
     </row>
     <row r="111" spans="2:4">
       <c r="B111" s="1" t="s">
-        <v>58</v>
+        <v>153</v>
       </c>
       <c r="C111" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="D111" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="112" spans="2:4">
       <c r="B112" s="1" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="C112" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
       <c r="D112" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="113" spans="2:4">
       <c r="B113" s="1" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C113" t="s">
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="D113" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="114" spans="2:4">
       <c r="B114" s="1" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="C114" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="D114" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="115" spans="2:4">
       <c r="B115" s="1" t="s">
-        <v>50</v>
+        <v>155</v>
       </c>
       <c r="C115" t="s">
-        <v>102</v>
+        <v>159</v>
       </c>
       <c r="D115" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="116" spans="2:4">
-      <c r="B116" s="1" t="s">
-        <v>56</v>
+      <c r="B116" t="s">
+        <v>290</v>
       </c>
       <c r="C116" t="s">
-        <v>103</v>
+        <v>294</v>
       </c>
       <c r="D116" t="s">
-        <v>137</v>
+        <v>295</v>
       </c>
     </row>
     <row r="117" spans="2:4">
-      <c r="B117" s="1" t="s">
-        <v>18</v>
+      <c r="B117" t="s">
+        <v>291</v>
       </c>
       <c r="C117" t="s">
-        <v>104</v>
+        <v>298</v>
       </c>
       <c r="D117" t="s">
-        <v>137</v>
+        <v>295</v>
       </c>
     </row>
     <row r="118" spans="2:4">
-      <c r="B118" s="1" t="s">
-        <v>57</v>
+      <c r="B118" t="s">
+        <v>292</v>
       </c>
       <c r="C118" t="s">
-        <v>105</v>
+        <v>296</v>
       </c>
       <c r="D118" t="s">
-        <v>137</v>
+        <v>295</v>
       </c>
     </row>
     <row r="119" spans="2:4">
       <c r="B119" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C119" t="s">
-        <v>113</v>
+        <v>144</v>
       </c>
       <c r="D119" t="s">
         <v>137</v>
@@ -6957,10 +7160,10 @@
     </row>
     <row r="120" spans="2:4">
       <c r="B120" s="1" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="C120" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="D120" t="s">
         <v>137</v>
@@ -6968,10 +7171,10 @@
     </row>
     <row r="121" spans="2:4">
       <c r="B121" s="1" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="C121" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="D121" t="s">
         <v>137</v>
@@ -6979,10 +7182,10 @@
     </row>
     <row r="122" spans="2:4">
       <c r="B122" s="1" t="s">
-        <v>322</v>
+        <v>22</v>
       </c>
       <c r="C122" t="s">
-        <v>325</v>
+        <v>101</v>
       </c>
       <c r="D122" t="s">
         <v>137</v>
@@ -6990,153 +7193,153 @@
     </row>
     <row r="123" spans="2:4">
       <c r="B123" s="1" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="C123" t="s">
-        <v>146</v>
+        <v>102</v>
       </c>
       <c r="D123" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="124" spans="2:4">
       <c r="B124" s="1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C124" t="s">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="D124" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
     </row>
     <row r="125" spans="2:4">
       <c r="B125" s="1" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="C125" t="s">
-        <v>82</v>
+        <v>104</v>
       </c>
       <c r="D125" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
     </row>
     <row r="126" spans="2:4">
       <c r="B126" s="1" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="C126" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="D126" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
     </row>
     <row r="127" spans="2:4">
       <c r="B127" s="1" t="s">
-        <v>187</v>
+        <v>62</v>
       </c>
       <c r="C127" t="s">
-        <v>213</v>
+        <v>113</v>
       </c>
       <c r="D127" t="s">
-        <v>214</v>
+        <v>137</v>
       </c>
     </row>
     <row r="128" spans="2:4">
-      <c r="B128" t="s">
-        <v>273</v>
+      <c r="B128" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="C128" t="s">
-        <v>283</v>
+        <v>115</v>
       </c>
       <c r="D128" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
     </row>
     <row r="129" spans="2:4">
-      <c r="B129" t="s">
-        <v>252</v>
+      <c r="B129" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="C129" t="s">
-        <v>253</v>
+        <v>122</v>
       </c>
       <c r="D129" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
     </row>
     <row r="130" spans="2:4">
-      <c r="B130" t="s">
-        <v>248</v>
+      <c r="B130" s="1" t="s">
+        <v>322</v>
       </c>
       <c r="C130" t="s">
-        <v>249</v>
+        <v>325</v>
       </c>
       <c r="D130" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
     </row>
     <row r="131" spans="2:4">
-      <c r="B131" t="s">
-        <v>258</v>
+      <c r="B131" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C131" t="s">
-        <v>259</v>
+        <v>146</v>
       </c>
       <c r="D131" t="s">
-        <v>132</v>
+        <v>147</v>
       </c>
     </row>
     <row r="132" spans="2:4">
-      <c r="B132" t="s">
-        <v>274</v>
+      <c r="B132" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="C132" t="s">
-        <v>284</v>
+        <v>79</v>
       </c>
       <c r="D132" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="133" spans="2:4">
-      <c r="B133" t="s">
-        <v>272</v>
+      <c r="B133" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="C133" t="s">
-        <v>282</v>
+        <v>82</v>
       </c>
       <c r="D133" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="134" spans="2:4">
       <c r="B134" s="1" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="C134" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="D134" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="135" spans="2:4">
       <c r="B135" s="1" t="s">
-        <v>229</v>
+        <v>187</v>
       </c>
       <c r="C135" t="s">
-        <v>232</v>
+        <v>213</v>
       </c>
       <c r="D135" t="s">
-        <v>132</v>
+        <v>214</v>
       </c>
     </row>
     <row r="136" spans="2:4">
       <c r="B136" t="s">
-        <v>300</v>
+        <v>273</v>
       </c>
       <c r="C136" t="s">
-        <v>301</v>
+        <v>283</v>
       </c>
       <c r="D136" t="s">
         <v>132</v>
@@ -7144,10 +7347,10 @@
     </row>
     <row r="137" spans="2:4">
       <c r="B137" t="s">
-        <v>310</v>
+        <v>252</v>
       </c>
       <c r="C137" t="s">
-        <v>312</v>
+        <v>253</v>
       </c>
       <c r="D137" t="s">
         <v>132</v>
@@ -7155,49 +7358,117 @@
     </row>
     <row r="138" spans="2:4">
       <c r="B138" t="s">
-        <v>314</v>
+        <v>248</v>
       </c>
       <c r="C138" t="s">
-        <v>319</v>
+        <v>249</v>
       </c>
       <c r="D138" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="139" spans="2:4">
-      <c r="B139" s="24" t="s">
+      <c r="B139" t="s">
+        <v>258</v>
+      </c>
+      <c r="C139" t="s">
+        <v>259</v>
+      </c>
+      <c r="D139" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="140" spans="2:4">
+      <c r="B140" t="s">
+        <v>274</v>
+      </c>
+      <c r="C140" t="s">
+        <v>284</v>
+      </c>
+      <c r="D140" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="141" spans="2:4">
+      <c r="B141" t="s">
+        <v>272</v>
+      </c>
+      <c r="C141" t="s">
+        <v>282</v>
+      </c>
+      <c r="D141" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="142" spans="2:4">
+      <c r="B142" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C142" t="s">
+        <v>111</v>
+      </c>
+      <c r="D142" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="143" spans="2:4">
+      <c r="B143" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C143" t="s">
+        <v>232</v>
+      </c>
+      <c r="D143" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="144" spans="2:4">
+      <c r="B144" t="s">
+        <v>300</v>
+      </c>
+      <c r="C144" t="s">
+        <v>301</v>
+      </c>
+      <c r="D144" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="145" spans="2:4">
+      <c r="B145" t="s">
+        <v>310</v>
+      </c>
+      <c r="C145" t="s">
+        <v>312</v>
+      </c>
+      <c r="D145" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="146" spans="2:4">
+      <c r="B146" t="s">
+        <v>314</v>
+      </c>
+      <c r="C146" t="s">
+        <v>319</v>
+      </c>
+      <c r="D146" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="147" spans="2:4">
+      <c r="B147" s="24" t="s">
         <v>328</v>
       </c>
-      <c r="C139" s="24" t="s">
+      <c r="C147" s="24" t="s">
         <v>329</v>
       </c>
-      <c r="D139" s="24" t="s">
+      <c r="D147" s="24" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="141" spans="2:4">
-      <c r="B141" s="23"/>
-      <c r="C141" s="24"/>
-      <c r="D141" s="24"/>
-    </row>
-    <row r="142" spans="2:4">
-      <c r="B142" s="23"/>
-      <c r="C142" s="24"/>
-      <c r="D142" s="24"/>
-    </row>
-    <row r="143" spans="2:4">
-      <c r="B143" s="23"/>
-      <c r="C143" s="24"/>
-      <c r="D143" s="24"/>
-    </row>
-    <row r="144" spans="2:4">
-      <c r="B144" s="23"/>
-      <c r="C144" s="24"/>
-      <c r="D144" s="24"/>
-    </row>
   </sheetData>
-  <sortState ref="B4:D139">
-    <sortCondition ref="D4:D139"/>
+  <sortState ref="B4:D147">
+    <sortCondition ref="D4:D147"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>